<commit_message>
created main use os.system
</commit_message>
<xml_diff>
--- a/database/SpotData.xlsx
+++ b/database/SpotData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="136">
   <si>
     <t>日期</t>
   </si>
@@ -421,6 +421,9 @@
   <si>
     <t>20180212</t>
   </si>
+  <si>
+    <t>20180213</t>
+  </si>
 </sst>
 </file>
 
@@ -768,7 +771,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AT91"/>
+  <dimension ref="A1:AT92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13513,6 +13516,146 @@
         <v>2417.27</v>
       </c>
     </row>
+    <row r="92" spans="1:46">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>135</v>
+      </c>
+      <c r="C92" t="n">
+        <v>51690</v>
+      </c>
+      <c r="D92" t="n">
+        <v>3924</v>
+      </c>
+      <c r="E92" t="n">
+        <v>26410</v>
+      </c>
+      <c r="F92" t="n">
+        <v>14120</v>
+      </c>
+      <c r="G92" t="n">
+        <v>270.58</v>
+      </c>
+      <c r="H92" t="n">
+        <v>4231.11</v>
+      </c>
+      <c r="I92" t="n">
+        <v>3963.33</v>
+      </c>
+      <c r="J92" t="n">
+        <v>11727.3</v>
+      </c>
+      <c r="K92" t="n">
+        <v>19050</v>
+      </c>
+      <c r="L92" t="n">
+        <v>3629.33</v>
+      </c>
+      <c r="M92" t="n">
+        <v>2843.33</v>
+      </c>
+      <c r="N92" t="n">
+        <v>4120.77</v>
+      </c>
+      <c r="O92" t="n">
+        <v>100300</v>
+      </c>
+      <c r="P92" t="n">
+        <v>146750</v>
+      </c>
+      <c r="Q92" t="n">
+        <v>5663.64</v>
+      </c>
+      <c r="R92" t="n">
+        <v>6262</v>
+      </c>
+      <c r="S92" t="n">
+        <v>15668</v>
+      </c>
+      <c r="T92" t="n">
+        <v>2538</v>
+      </c>
+      <c r="U92" t="n">
+        <v>6471.67</v>
+      </c>
+      <c r="V92" t="n">
+        <v>2613.33</v>
+      </c>
+      <c r="W92" t="n">
+        <v>1543.2</v>
+      </c>
+      <c r="X92" t="n">
+        <v>2335</v>
+      </c>
+      <c r="Y92" t="n">
+        <v>5490</v>
+      </c>
+      <c r="Z92" t="n">
+        <v>2998.33</v>
+      </c>
+      <c r="AA92" t="n">
+        <v>2710</v>
+      </c>
+      <c r="AB92" t="n">
+        <v>7204.55</v>
+      </c>
+      <c r="AC92" t="n">
+        <v>8131.25</v>
+      </c>
+      <c r="AD92" t="n">
+        <v>2855</v>
+      </c>
+      <c r="AE92" t="n">
+        <v>743.2</v>
+      </c>
+      <c r="AF92" t="n">
+        <v>5135</v>
+      </c>
+      <c r="AG92" t="n">
+        <v>6450</v>
+      </c>
+      <c r="AH92" t="n">
+        <v>9655</v>
+      </c>
+      <c r="AI92" t="n">
+        <v>3660</v>
+      </c>
+      <c r="AJ92" t="n">
+        <v>2938.75</v>
+      </c>
+      <c r="AK92" t="n">
+        <v>5600</v>
+      </c>
+      <c r="AL92" t="n">
+        <v>1780.36</v>
+      </c>
+      <c r="AM92" t="n">
+        <v>1880</v>
+      </c>
+      <c r="AN92" t="n">
+        <v>1498.33</v>
+      </c>
+      <c r="AO92" t="n">
+        <v>548.67</v>
+      </c>
+      <c r="AP92" t="n">
+        <v>4275</v>
+      </c>
+      <c r="AQ92" t="n">
+        <v>122.67</v>
+      </c>
+      <c r="AR92" t="n">
+        <v>75</v>
+      </c>
+      <c r="AS92" t="n">
+        <v>9175</v>
+      </c>
+      <c r="AT92" t="n">
+        <v>2417.27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>